<commit_message>
It works with opportunistic takeovers, and
</commit_message>
<xml_diff>
--- a/seed_band_1.xlsx
+++ b/seed_band_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23256" windowHeight="12588"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22560" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="52">
   <si>
     <t>Individual ID #</t>
   </si>
@@ -146,6 +146,33 @@
   </si>
   <si>
     <t>lea = 3, fol = 2, sol = 1, juvsol = 0</t>
+  </si>
+  <si>
+    <t>females if applicable</t>
+  </si>
+  <si>
+    <t>fols if applicable</t>
+  </si>
+  <si>
+    <t>50,52,54,55</t>
+  </si>
+  <si>
+    <t>59,61,62</t>
+  </si>
+  <si>
+    <t>41,44,46</t>
+  </si>
+  <si>
+    <t>31,33</t>
+  </si>
+  <si>
+    <t>19,22,25,28</t>
+  </si>
+  <si>
+    <t>12,15</t>
+  </si>
+  <si>
+    <t>3,6,8,10</t>
   </si>
 </sst>
 </file>
@@ -730,11 +757,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="215043072"/>
-        <c:axId val="215048960"/>
+        <c:axId val="213478400"/>
+        <c:axId val="213484288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="215043072"/>
+        <c:axId val="213478400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215048960"/>
+        <c:crossAx val="213484288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="215048960"/>
+        <c:axId val="213484288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215043072"/>
+        <c:crossAx val="213478400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1101,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,13 +1139,13 @@
     <col min="1" max="4" width="9.109375" style="1"/>
     <col min="5" max="5" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="7" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
@@ -1134,7 +1161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1156,14 +1183,20 @@
       <c r="G2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1186,15 +1219,21 @@
       <c r="G3" s="5">
         <v>3</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="33"/>
-    </row>
-    <row r="4" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="33"/>
+    </row>
+    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1218,12 +1257,12 @@
       <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -1244,13 +1283,13 @@
       <c r="F5" s="5">
         <v>19.5</v>
       </c>
-      <c r="H5" s="3">
+      <c r="J5" s="3">
         <f>(36 / (65 - 36))</f>
         <v>1.2413793103448276</v>
       </c>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -1275,11 +1314,11 @@
       <c r="G6" s="5">
         <v>0</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1300,12 +1339,12 @@
       <c r="F7" s="5">
         <v>0.5</v>
       </c>
-      <c r="H7" s="20" t="e">
+      <c r="J7" s="20" t="e">
         <f>(36- SUM(#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!))/SUM(#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1326,11 +1365,11 @@
       <c r="F8" s="5">
         <v>12</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -1351,11 +1390,11 @@
       <c r="F9" s="5">
         <v>0</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -1377,7 +1416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -1399,7 +1438,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>1</v>
       </c>
@@ -1421,7 +1460,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>1</v>
       </c>
@@ -1445,17 +1484,20 @@
       <c r="G13" s="17">
         <v>3</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="H13" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
-      <c r="S13" s="5"/>
-    </row>
-    <row r="14" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="U13" s="5"/>
+    </row>
+    <row r="14" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>1</v>
       </c>
@@ -1476,15 +1518,15 @@
       <c r="F14" s="17">
         <v>18.5</v>
       </c>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
       <c r="O14" s="34"/>
-      <c r="S14" s="5"/>
-    </row>
-    <row r="15" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="U14" s="5"/>
+    </row>
+    <row r="15" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>1</v>
       </c>
@@ -1505,15 +1547,15 @@
       <c r="F15" s="17">
         <v>3</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
       <c r="O15" s="34"/>
-      <c r="S15" s="5"/>
-    </row>
-    <row r="16" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="U15" s="5"/>
+    </row>
+    <row r="16" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>1</v>
       </c>
@@ -1534,15 +1576,15 @@
       <c r="F16" s="17">
         <v>0</v>
       </c>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
       <c r="O16" s="34"/>
-      <c r="S16" s="5"/>
-    </row>
-    <row r="17" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="U16" s="5"/>
+    </row>
+    <row r="17" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>1</v>
       </c>
@@ -1563,15 +1605,15 @@
       <c r="F17" s="17">
         <v>13</v>
       </c>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
       <c r="O17" s="34"/>
-      <c r="S17" s="5"/>
-    </row>
-    <row r="18" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="U17" s="5"/>
+    </row>
+    <row r="18" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>1</v>
       </c>
@@ -1592,15 +1634,15 @@
       <c r="F18" s="17">
         <v>0.5</v>
       </c>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
       <c r="O18" s="34"/>
-      <c r="S18" s="5"/>
-    </row>
-    <row r="19" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="U18" s="5"/>
+    </row>
+    <row r="19" spans="1:21" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>2</v>
       </c>
@@ -1624,15 +1666,21 @@
       <c r="G19" s="15">
         <v>3</v>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
+      <c r="H19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="15">
+        <v>18</v>
+      </c>
       <c r="L19" s="34"/>
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
       <c r="O19" s="34"/>
-      <c r="S19" s="5"/>
-    </row>
-    <row r="20" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="U19" s="5"/>
+    </row>
+    <row r="20" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>2</v>
       </c>
@@ -1656,15 +1704,15 @@
       <c r="G20" s="15">
         <v>2</v>
       </c>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
       <c r="L20" s="34"/>
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
       <c r="O20" s="34"/>
-      <c r="S20" s="5"/>
-    </row>
-    <row r="21" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="U20" s="5"/>
+    </row>
+    <row r="21" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>2</v>
       </c>
@@ -1685,15 +1733,15 @@
       <c r="F21" s="15">
         <v>11.5</v>
       </c>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
       <c r="L21" s="34"/>
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
       <c r="O21" s="34"/>
-      <c r="S21" s="5"/>
-    </row>
-    <row r="22" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="U21" s="5"/>
+    </row>
+    <row r="22" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>2</v>
       </c>
@@ -1714,9 +1762,9 @@
       <c r="F22" s="24">
         <v>0</v>
       </c>
-      <c r="S22" s="5"/>
-    </row>
-    <row r="23" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U22" s="5"/>
+    </row>
+    <row r="23" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>2</v>
       </c>
@@ -1737,19 +1785,19 @@
       <c r="F23" s="24">
         <v>2</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="K23" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
       <c r="L23" s="35"/>
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
       <c r="O23" s="35"/>
       <c r="P23" s="35"/>
-      <c r="S23" s="5"/>
-    </row>
-    <row r="24" spans="1:19" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="U23" s="5"/>
+    </row>
+    <row r="24" spans="1:21" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>2</v>
       </c>
@@ -1770,21 +1818,21 @@
       <c r="F24" s="15">
         <v>12</v>
       </c>
-      <c r="I24" s="35" t="s">
+      <c r="K24" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
       <c r="L24" s="35"/>
-      <c r="M24" s="35" t="s">
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
       <c r="P24" s="35"/>
-      <c r="S24" s="5"/>
-    </row>
-    <row r="25" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="U24" s="5"/>
+    </row>
+    <row r="25" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>2</v>
       </c>
@@ -1808,17 +1856,17 @@
       <c r="G25" s="15">
         <v>0</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="K25" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35" t="s">
+      <c r="L25" s="35"/>
+      <c r="M25" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="L25" s="35"/>
-      <c r="S25" s="5"/>
-    </row>
-    <row r="26" spans="1:19" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="35"/>
+      <c r="U25" s="5"/>
+    </row>
+    <row r="26" spans="1:21" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>2</v>
       </c>
@@ -1839,15 +1887,15 @@
       <c r="F26" s="15">
         <v>0.5</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="K26" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="L26" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="S26" s="5"/>
-    </row>
-    <row r="27" spans="1:19" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U26" s="5"/>
+    </row>
+    <row r="27" spans="1:21" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>2</v>
       </c>
@@ -1868,39 +1916,39 @@
       <c r="F27" s="15">
         <v>12</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="K27" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="L27" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="M27" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L27" s="15" t="s">
+      <c r="N27" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M27" s="15" t="s">
+      <c r="O27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="N27" s="15" t="s">
+      <c r="P27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="15" t="s">
+      <c r="Q27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="P27" s="15" t="s">
+      <c r="R27" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="Q27" s="15" t="s">
+      <c r="S27" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="R27" s="15" t="s">
+      <c r="T27" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="S27" s="5"/>
-    </row>
-    <row r="28" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U27" s="5"/>
+    </row>
+    <row r="28" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>2</v>
       </c>
@@ -1921,12 +1969,6 @@
       <c r="F28" s="24">
         <v>2.5</v>
       </c>
-      <c r="I28" s="22">
-        <v>0.125</v>
-      </c>
-      <c r="J28" s="22">
-        <v>0.125</v>
-      </c>
       <c r="K28" s="22">
         <v>0.125</v>
       </c>
@@ -1934,10 +1976,10 @@
         <v>0.125</v>
       </c>
       <c r="M28" s="22">
-        <v>8.3000000000000004E-2</v>
+        <v>0.125</v>
       </c>
       <c r="N28" s="22">
-        <v>8.3000000000000004E-2</v>
+        <v>0.125</v>
       </c>
       <c r="O28" s="22">
         <v>8.3000000000000004E-2</v>
@@ -1951,9 +1993,15 @@
       <c r="R28" s="22">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="S28" s="5"/>
-    </row>
-    <row r="29" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S28" s="22">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="T28" s="22">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="U28" s="5"/>
+    </row>
+    <row r="29" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>2</v>
       </c>
@@ -1974,9 +2022,9 @@
       <c r="F29" s="24">
         <v>1</v>
       </c>
-      <c r="S29" s="5"/>
-    </row>
-    <row r="30" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U29" s="5"/>
+    </row>
+    <row r="30" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <v>2</v>
       </c>
@@ -1997,9 +2045,9 @@
       <c r="F30" s="15">
         <v>6</v>
       </c>
-      <c r="S30" s="5"/>
-    </row>
-    <row r="31" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>2</v>
       </c>
@@ -2020,9 +2068,9 @@
       <c r="F31" s="15">
         <v>0</v>
       </c>
-      <c r="S31" s="5"/>
-    </row>
-    <row r="32" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U31" s="5"/>
+    </row>
+    <row r="32" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>2</v>
       </c>
@@ -2046,9 +2094,12 @@
       <c r="G32" s="9">
         <v>3</v>
       </c>
-      <c r="S32" s="5"/>
-    </row>
-    <row r="33" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U32" s="5"/>
+    </row>
+    <row r="33" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>2</v>
       </c>
@@ -2069,9 +2120,9 @@
       <c r="F33" s="9">
         <v>5</v>
       </c>
-      <c r="S33" s="5"/>
-    </row>
-    <row r="34" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U33" s="5"/>
+    </row>
+    <row r="34" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>2</v>
       </c>
@@ -2092,9 +2143,9 @@
       <c r="F34" s="9">
         <v>0</v>
       </c>
-      <c r="S34" s="5"/>
-    </row>
-    <row r="35" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U34" s="5"/>
+    </row>
+    <row r="35" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>2</v>
       </c>
@@ -2115,9 +2166,9 @@
       <c r="F35" s="9">
         <v>12</v>
       </c>
-      <c r="S35" s="5"/>
-    </row>
-    <row r="36" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U35" s="5"/>
+    </row>
+    <row r="36" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>2</v>
       </c>
@@ -2138,9 +2189,9 @@
       <c r="F36" s="26">
         <v>2</v>
       </c>
-      <c r="S36" s="5"/>
-    </row>
-    <row r="37" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U36" s="5"/>
+    </row>
+    <row r="37" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -2161,9 +2212,9 @@
       <c r="F37" s="26">
         <v>0.5</v>
       </c>
-      <c r="S37" s="5"/>
-    </row>
-    <row r="38" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U37" s="5"/>
+    </row>
+    <row r="38" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>2</v>
       </c>
@@ -2187,9 +2238,12 @@
       <c r="G38" s="19">
         <v>3</v>
       </c>
-      <c r="S38" s="5"/>
-    </row>
-    <row r="39" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H38" s="19">
+        <v>37</v>
+      </c>
+      <c r="U38" s="5"/>
+    </row>
+    <row r="39" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>2</v>
       </c>
@@ -2210,9 +2264,9 @@
       <c r="F39" s="19">
         <v>19</v>
       </c>
-      <c r="S39" s="5"/>
-    </row>
-    <row r="40" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U39" s="5"/>
+    </row>
+    <row r="40" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>2</v>
       </c>
@@ -2235,7 +2289,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="41" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>2</v>
       </c>
@@ -2257,7 +2311,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2</v>
       </c>
@@ -2279,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>3</v>
       </c>
@@ -2303,8 +2357,11 @@
       <c r="G43" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H43" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <v>3</v>
       </c>
@@ -2326,7 +2383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
         <v>3</v>
       </c>
@@ -2351,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>3</v>
       </c>
@@ -2373,7 +2430,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>3</v>
       </c>
@@ -2395,7 +2452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>3</v>
       </c>
@@ -2417,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>3</v>
       </c>
@@ -2439,7 +2496,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <v>3</v>
       </c>
@@ -2461,7 +2518,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>3</v>
       </c>
@@ -2483,7 +2540,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>3</v>
       </c>
@@ -2507,8 +2564,11 @@
       <c r="G52" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H52" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>3</v>
       </c>
@@ -2530,7 +2590,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>3</v>
       </c>
@@ -2552,7 +2612,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>3</v>
       </c>
@@ -2574,7 +2634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>3</v>
       </c>
@@ -2596,7 +2656,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>3</v>
       </c>
@@ -2618,7 +2678,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>3</v>
       </c>
@@ -2640,7 +2700,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>3</v>
       </c>
@@ -2662,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>3</v>
       </c>
@@ -2686,8 +2746,14 @@
       <c r="G60" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H60" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" s="7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>3</v>
       </c>
@@ -2712,7 +2778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>3</v>
       </c>
@@ -2734,7 +2800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>3</v>
       </c>
@@ -2756,7 +2822,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>3</v>
       </c>
@@ -2860,13 +2926,13 @@
   <mergeCells count="9">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="J2:J5"/>
-    <mergeCell ref="J13:O21"/>
-    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="L13:Q21"/>
     <mergeCell ref="K25:L25"/>
-    <mergeCell ref="I23:P23"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="O24:R24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>